<commit_message>
Add external variables to pilot
- add init time, type and callsgin mathcing to pilot
- add invalid initialization type check
-
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\03_Konzepterarbeitung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF3EAA0-95E5-4E81-84A6-705F2005DA77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B389A9F-D18C-4325-B4C7-16F6DF670E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
   <si>
     <t>Type</t>
   </si>
@@ -266,6 +266,27 @@
   </si>
   <si>
     <t>gravitional constant</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>[Landing, Takeoff]</t>
+  </si>
+  <si>
+    <t>time_initialization</t>
+  </si>
+  <si>
+    <t>[2; inf]</t>
+  </si>
+  <si>
+    <t>Defines</t>
+  </si>
+  <si>
+    <t>Defines whether this pilot is going to be landing or starting from ground</t>
+  </si>
+  <si>
+    <t>type_initialization</t>
   </si>
 </sst>
 </file>
@@ -756,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66623BDC-BB60-4807-9757-51D95C0437E4}">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1297,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1344,111 +1365,101 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="5" t="s">
+    <row r="9" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B9" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
@@ -1463,9 +1474,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
@@ -1482,7 +1493,7 @@
     </row>
     <row r="13" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
@@ -1499,191 +1510,242 @@
     </row>
     <row r="14" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add all reasonable external variables for aircraft
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542A32C-FC88-4857-82C1-59C4BE3ADECC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD7E83-09E4-43C5-91CC-B532662383B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
     <sheet name="Observer" sheetId="2" r:id="rId2"/>
     <sheet name="Pilot" sheetId="3" r:id="rId3"/>
+    <sheet name="Aircraft" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="168">
   <si>
     <t>Type</t>
   </si>
@@ -292,10 +293,253 @@
     <t>[1; inf]</t>
   </si>
   <si>
-    <t>Defines the starting time of the pilot AND ist aircraft</t>
-  </si>
-  <si>
     <t>Callsign number, that has to match a callsign number of the aircraft variables table</t>
+  </si>
+  <si>
+    <t>Defines the starting time of the pilot AND its aircraft</t>
+  </si>
+  <si>
+    <t>Callsign number, that has to match a callsign number of the pilot variables table</t>
+  </si>
+  <si>
+    <t>Aircraft__mass</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>[550; 725]</t>
+  </si>
+  <si>
+    <t>Aircraft__wing_area</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>[15]</t>
+  </si>
+  <si>
+    <t>Aircraft__wing_span</t>
+  </si>
+  <si>
+    <t>[10.1]</t>
+  </si>
+  <si>
+    <t>Aircraft__stall_angle</t>
+  </si>
+  <si>
+    <t>Aircraft__lift_coefficient_slope</t>
+  </si>
+  <si>
+    <t>[4.9]</t>
+  </si>
+  <si>
+    <t>Aircraft__zero_lift_angle</t>
+  </si>
+  <si>
+    <t>Aircraft__total_stall_angle</t>
+  </si>
+  <si>
+    <t>[-1.0]</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>Defines the angle when complete flow separation occurs and now lift will be produced</t>
+  </si>
+  <si>
+    <t>Aircraft__zero_lift_drag_coefficient</t>
+  </si>
+  <si>
+    <t>[0.04]</t>
+  </si>
+  <si>
+    <t>Aircraft__oswald_factor</t>
+  </si>
+  <si>
+    <t>[0.7]</t>
+  </si>
+  <si>
+    <t>Typical value for small single engine aircraft, fixed gear</t>
+  </si>
+  <si>
+    <t>Brake__deceleration_force_max</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>[2500; 3000]</t>
+  </si>
+  <si>
+    <t>Simplified maximum brake force</t>
+  </si>
+  <si>
+    <t>Propeller__diameter</t>
+  </si>
+  <si>
+    <t>[1.75]</t>
+  </si>
+  <si>
+    <t>[-0.002]</t>
+  </si>
+  <si>
+    <t>Propeller__thrust_coefficient_slope</t>
+  </si>
+  <si>
+    <t>Propeller__thrust_coefficient_constant</t>
+  </si>
+  <si>
+    <t>[0.1]</t>
+  </si>
+  <si>
+    <t>Propeller__thrust_coefficient_speed_constant</t>
+  </si>
+  <si>
+    <t>[25]</t>
+  </si>
+  <si>
+    <t>Up to which speed the "Propeller__thrust_coefficient_constant" is constant</t>
+  </si>
+  <si>
+    <t>Engine__power_coefficient_slope</t>
+  </si>
+  <si>
+    <t>[-0.0009]</t>
+  </si>
+  <si>
+    <t>Engine__power_coefficient_constant</t>
+  </si>
+  <si>
+    <t>Engine__power_coefficient_speed_constant</t>
+  </si>
+  <si>
+    <t>[0.05]</t>
+  </si>
+  <si>
+    <t>[30.0]</t>
+  </si>
+  <si>
+    <t>Up to which speed the "Engine__power_coefficient_constant" is constant</t>
+  </si>
+  <si>
+    <t>Engine__RPM_max</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>[2750]</t>
+  </si>
+  <si>
+    <t>Maximum mechanical revolution per minute</t>
+  </si>
+  <si>
+    <t>Engine__power_max</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>[75000]</t>
+  </si>
+  <si>
+    <t>Engine__fuel_consumption_max</t>
+  </si>
+  <si>
+    <t>l/s</t>
+  </si>
+  <si>
+    <t>[0.0079]</t>
+  </si>
+  <si>
+    <t>Engine__oil_pump_condition_probability</t>
+  </si>
+  <si>
+    <t>Probability of oil pump condition to be healthy</t>
+  </si>
+  <si>
+    <t>Engine__oil_leakage_probability</t>
+  </si>
+  <si>
+    <t>Probability of an engine oil leakage</t>
+  </si>
+  <si>
+    <t>Engine__failure_probability_add_water_sediments</t>
+  </si>
+  <si>
+    <t>Engine__failure_probability_add_oil_min</t>
+  </si>
+  <si>
+    <t>Engine__failure_probability_add_oil_critical_min</t>
+  </si>
+  <si>
+    <t>Engine__failure_probability_add_oil_pump_condition</t>
+  </si>
+  <si>
+    <t>Probability of an engine failure (per each tick!) due to water sediments</t>
+  </si>
+  <si>
+    <t>Probability of an engine failure (per each tick!) due to enigne oil below minimum</t>
+  </si>
+  <si>
+    <t>Probability of an engine failure (per each tick!) due to engine oil below critical minimum</t>
+  </si>
+  <si>
+    <t>Probability of an engine failure (per each tick!) due to faulty engine pump condition</t>
+  </si>
+  <si>
+    <t>RWT__total_capacity</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>[49]</t>
+  </si>
+  <si>
+    <t>Right wing fuel tank capacity</t>
+  </si>
+  <si>
+    <t>RWT__water_sediments_probability</t>
+  </si>
+  <si>
+    <t>Probability of existing water sediments in the right wing tank</t>
+  </si>
+  <si>
+    <t>LWT__total_capacity</t>
+  </si>
+  <si>
+    <t>Light wing fuel tank capacity</t>
+  </si>
+  <si>
+    <t>LWT__water_sediments_probability</t>
+  </si>
+  <si>
+    <t>Probability of existing water sediments in the left wing tank</t>
+  </si>
+  <si>
+    <t>Tire__wheel_radius</t>
+  </si>
+  <si>
+    <t>[0.075]</t>
+  </si>
+  <si>
+    <t>Wheel diameter with neglecting non equal size of nose and main wheels</t>
+  </si>
+  <si>
+    <t>Tire__roll_coefficient</t>
+  </si>
+  <si>
+    <t>[0.002]</t>
+  </si>
+  <si>
+    <t>For the calculation of the friction</t>
+  </si>
+  <si>
+    <t>Fuel consumption for 100% throttle (correspond to 7.5 gallon per hour)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +712,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1329,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1405,7 +1661,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
@@ -1422,7 +1678,7 @@
         <v>84</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
@@ -1773,4 +2029,833 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A179EA-4F63-4261-A653-91ADE6AC0E5C}">
+  <dimension ref="A1:F63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.19921875" customWidth="1"/>
+    <col min="2" max="2" width="49.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.73046875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="53.19921875" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="4"/>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="2:6" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B23" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B31" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B32" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B33" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B34" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B35" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="3"/>
+      <c r="B36" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="3"/>
+      <c r="B37" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{CF6B7080-DDAE-4369-8024-11059A5D83DB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Add external variable for crash detection
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD7E83-09E4-43C5-91CC-B532662383B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107AF0A0-003E-4CA0-B2E8-23E646B4A8DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="171">
   <si>
     <t>Type</t>
   </si>
@@ -540,6 +540,15 @@
   </si>
   <si>
     <t>Fuel consumption for 100% throttle (correspond to 7.5 gallon per hour)</t>
+  </si>
+  <si>
+    <t>Taxiing__collision_crash_distance</t>
+  </si>
+  <si>
+    <t>[1; 3]</t>
+  </si>
+  <si>
+    <t>Distance threshold for crash detecion</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1988,11 +1997,21 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="5"/>
@@ -2035,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A179EA-4F63-4261-A653-91ADE6AC0E5C}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add n_cycle to external varibles
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107AF0A0-003E-4CA0-B2E8-23E646B4A8DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56C716C-AA2E-4D82-9DB8-3EF2C0170B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="174">
   <si>
     <t>Type</t>
   </si>
@@ -549,6 +549,15 @@
   </si>
   <si>
     <t>Distance threshold for crash detecion</t>
+  </si>
+  <si>
+    <t>n_cycle</t>
+  </si>
+  <si>
+    <t>[1; 100]</t>
+  </si>
+  <si>
+    <t>Defines the number of calculation cycles between each tick for the numerical calculation of the aircraft physics (low numbers might lead to unstable behaviour)</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -2054,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A179EA-4F63-4261-A653-91ADE6AC0E5C}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2662,13 +2671,23 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>

</xml_diff>

<commit_message>
Fix spelling or sort variables overview
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56C716C-AA2E-4D82-9DB8-3EF2C0170B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E36AF8-CA68-49B2-8D11-6E7ED6190134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -89,12 +89,6 @@
     <t>[0; 360]</t>
   </si>
   <si>
-    <t>[0; inf]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-273,15; inf]  </t>
-  </si>
-  <si>
     <t>Outside air temperature at airport</t>
   </si>
   <si>
@@ -263,9 +257,6 @@
     <t>m/s^2</t>
   </si>
   <si>
-    <t>~9.81</t>
-  </si>
-  <si>
     <t>gravitional constant</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Callsign number, that has to match a callsign number of the aircraft variables table</t>
   </si>
   <si>
-    <t>Defines the starting time of the pilot AND its aircraft</t>
-  </si>
-  <si>
     <t>Callsign number, that has to match a callsign number of the pilot variables table</t>
   </si>
   <si>
@@ -347,9 +335,6 @@
     <t>[11]</t>
   </si>
   <si>
-    <t>Defines the angle when complete flow separation occurs and now lift will be produced</t>
-  </si>
-  <si>
     <t>Aircraft__zero_lift_drag_coefficient</t>
   </si>
   <si>
@@ -458,15 +443,9 @@
     <t>Engine__oil_pump_condition_probability</t>
   </si>
   <si>
-    <t>Probability of oil pump condition to be healthy</t>
-  </si>
-  <si>
     <t>Engine__oil_leakage_probability</t>
   </si>
   <si>
-    <t>Probability of an engine oil leakage</t>
-  </si>
-  <si>
     <t>Engine__failure_probability_add_water_sediments</t>
   </si>
   <si>
@@ -506,9 +485,6 @@
     <t>RWT__water_sediments_probability</t>
   </si>
   <si>
-    <t>Probability of existing water sediments in the right wing tank</t>
-  </si>
-  <si>
     <t>LWT__total_capacity</t>
   </si>
   <si>
@@ -518,9 +494,6 @@
     <t>LWT__water_sediments_probability</t>
   </si>
   <si>
-    <t>Probability of existing water sediments in the left wing tank</t>
-  </si>
-  <si>
     <t>Tire__wheel_radius</t>
   </si>
   <si>
@@ -539,9 +512,6 @@
     <t>For the calculation of the friction</t>
   </si>
   <si>
-    <t>Fuel consumption for 100% throttle (correspond to 7.5 gallon per hour)</t>
-  </si>
-  <si>
     <t>Taxiing__collision_crash_distance</t>
   </si>
   <si>
@@ -558,6 +528,36 @@
   </si>
   <si>
     <t>Defines the number of calculation cycles between each tick for the numerical calculation of the aircraft physics (low numbers might lead to unstable behaviour)</t>
+  </si>
+  <si>
+    <t>Defines the starting time of the pilot AND its aircraft. Please do NOT use the same time twice, since spawning might be unstable. Please choose a reasonable high delta between landing aircrafts.</t>
+  </si>
+  <si>
+    <t>Probability of existing water sediments in the left wing tank during initialization</t>
+  </si>
+  <si>
+    <t>Probability of existing water sediments in the right wing tank during initialization</t>
+  </si>
+  <si>
+    <t>Probability of an engine oil leakage during initialization</t>
+  </si>
+  <si>
+    <t>Probability of oil pump condition to be healthy during initialization</t>
+  </si>
+  <si>
+    <t>[9.81]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-10; 50]  </t>
+  </si>
+  <si>
+    <t>[0; 15]</t>
+  </si>
+  <si>
+    <t>Fuel consumption for 100% throttle (corresponds to 7.5 gallon per hour)</t>
+  </si>
+  <si>
+    <t>Defines the angle when complete flow separation occurs and no lift will be produced</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,6 +742,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1061,7 +1064,7 @@
   <dimension ref="B1:F31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1106,36 +1109,36 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>169</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
@@ -1149,44 +1152,44 @@
         <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
@@ -1344,6 +1347,9 @@
       <c r="F31" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F9">
+    <sortCondition ref="B4"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{70A8C597-2495-4536-87C8-B97DFF128933}"/>
   </hyperlinks>
@@ -1404,36 +1410,36 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
@@ -1603,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1650,160 +1656,160 @@
     </row>
     <row r="5" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
@@ -1812,214 +1818,214 @@
         <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>158</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>169</v>
+        <v>75</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
@@ -2051,6 +2057,9 @@
       <c r="F30" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F26">
+    <sortCondition ref="B4"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{3C4D1320-15C9-4AA0-851F-8D07A8F1D73D}"/>
   </hyperlinks>
@@ -2063,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A179EA-4F63-4261-A653-91ADE6AC0E5C}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2108,35 +2117,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>13</v>
@@ -2144,16 +2153,16 @@
     </row>
     <row r="7" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>13</v>
@@ -2161,22 +2170,22 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
         <v>96</v>
       </c>
@@ -2187,24 +2196,24 @@
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -2212,24 +2221,24 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
@@ -2238,15 +2247,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
@@ -2255,134 +2264,134 @@
         <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B17" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B18" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
@@ -2391,58 +2400,58 @@
         <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="5" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -2450,243 +2459,243 @@
     </row>
     <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>140</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>41</v>
+      <c r="B28" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>146</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>41</v>
+      <c r="B29" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>39</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B30" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B31" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>13</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>150</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B32" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>154</v>
+      <c r="B32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B33" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B34" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>158</v>
+      <c r="B33" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B34" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B35" s="19" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
-      <c r="B36" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>163</v>
+      <c r="B36" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="5" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -2890,6 +2899,9 @@
       <c r="F63" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F38">
+    <sortCondition ref="B4"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{CF6B7080-DDAE-4369-8024-11059A5D83DB}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Fix spelling and add comments
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E36AF8-CA68-49B2-8D11-6E7ED6190134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CDF14-96D3-4175-B173-6E4D9702C892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>m/s^2</t>
   </si>
   <si>
-    <t>gravitional constant</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -558,6 +555,9 @@
   </si>
   <si>
     <t>Defines the angle when complete flow separation occurs and no lift will be produced</t>
+  </si>
+  <si>
+    <t>Gravitational constant</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66623BDC-BB60-4807-9757-51D95C0437E4}">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1118,10 +1118,10 @@
         <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1152,7 +1152,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>17</v>
@@ -1186,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1609,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8244816A-1109-49C7-9A3A-8BED1BE383E9}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="5" spans="2:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>23</v>
@@ -1665,10 +1665,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -1877,7 +1877,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
@@ -1886,10 +1886,10 @@
         <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
@@ -1996,7 +1996,7 @@
     </row>
     <row r="25" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>23</v>
@@ -2005,27 +2005,27 @@
         <v>26</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="F26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
@@ -2119,16 +2119,16 @@
     </row>
     <row r="5" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -2136,16 +2136,16 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>13</v>
@@ -2153,16 +2153,16 @@
     </row>
     <row r="7" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>13</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -2179,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>13</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="9" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -2196,24 +2196,24 @@
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
@@ -2230,7 +2230,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>13</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
@@ -2247,7 +2247,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>13</v>
@@ -2255,41 +2255,41 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>23</v>
@@ -2298,15 +2298,15 @@
         <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B16" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>6</v>
@@ -2318,12 +2318,12 @@
         <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B17" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>6</v>
@@ -2335,12 +2335,12 @@
         <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B18" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>6</v>
@@ -2352,12 +2352,12 @@
         <v>39</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
@@ -2369,29 +2369,29 @@
         <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
@@ -2403,12 +2403,12 @@
         <v>39</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
@@ -2420,12 +2420,12 @@
         <v>39</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>6</v>
@@ -2434,7 +2434,7 @@
         <v>13</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>13</v>
@@ -2442,16 +2442,16 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="25" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
@@ -2468,24 +2468,24 @@
         <v>12</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -2493,41 +2493,41 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>146</v>
-      </c>
       <c r="F28" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>6</v>
@@ -2539,12 +2539,12 @@
         <v>39</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B30" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>23</v>
@@ -2553,15 +2553,15 @@
         <v>13</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B31" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>6</v>
@@ -2570,7 +2570,7 @@
         <v>33</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>13</v>
@@ -2578,16 +2578,16 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>13</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B33" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
@@ -2604,7 +2604,7 @@
         <v>13</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>13</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B34" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>6</v>
@@ -2621,33 +2621,33 @@
         <v>12</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B35" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="F35" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>6</v>
@@ -2659,13 +2659,13 @@
         <v>39</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
@@ -2674,16 +2674,16 @@
         <v>33</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
@@ -2692,10 +2692,10 @@
         <v>33</v>
       </c>
       <c r="E38" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Fix wrong value in table
</commit_message>
<xml_diff>
--- a/Variable_Overview.xlsx
+++ b/Variable_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eriks\Google Drive\Bachelorarbeit\02_Eclipse_Workspace\cessna_digital_twin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301CDF14-96D3-4175-B173-6E4D9702C892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F3E69-A1D4-4181-96D0-7E1778DCD686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{47946F22-9101-49D5-A5FC-082DA34A7C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather" sheetId="1" r:id="rId1"/>
@@ -503,9 +503,6 @@
     <t>Tire__roll_coefficient</t>
   </si>
   <si>
-    <t>[0.002]</t>
-  </si>
-  <si>
     <t>For the calculation of the friction</t>
   </si>
   <si>
@@ -558,6 +555,9 @@
   </si>
   <si>
     <t>Gravitational constant</t>
+  </si>
+  <si>
+    <t>[0.003]</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66623BDC-BB60-4807-9757-51D95C0437E4}">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1118,10 +1118,10 @@
         <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1152,7 +1152,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>17</v>
@@ -1186,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>13</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
@@ -1886,10 +1886,10 @@
         <v>33</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
@@ -2008,7 +2008,7 @@
         <v>76</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -2072,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A179EA-4F63-4261-A653-91ADE6AC0E5C}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2199,7 +2199,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
@@ -2386,7 +2386,7 @@
         <v>132</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
@@ -2403,7 +2403,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -2420,7 +2420,7 @@
         <v>39</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.45">
@@ -2539,12 +2539,12 @@
         <v>39</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B30" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>23</v>
@@ -2553,10 +2553,10 @@
         <v>13</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.45">
@@ -2659,7 +2659,7 @@
         <v>39</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -2674,10 +2674,10 @@
         <v>33</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">

</xml_diff>